<commit_message>
Completed xlsio functionality and docs
- Added functionality to indicate reverse biased cells. Reverse biased and bypassed cells are indicated on the same excel tab (assuming that a bypassed cell cannot be reverse biased).
- Added functionality of temperature input.
- Fixed imports and style.
- Updated README, example_workflow .py and .ipynb.
</commit_message>
<xml_diff>
--- a/pvmismatch/contrib/xlsio/example_workflow/ExcelLayoutFromPVMM.xlsx
+++ b/pvmismatch/contrib/xlsio/example_workflow/ExcelLayoutFromPVMM.xlsx
@@ -10,7 +10,7 @@
     <sheet name="CellIndexes" sheetId="1" r:id="rId1"/>
     <sheet name="Irradiance" sheetId="2" r:id="rId2"/>
     <sheet name="CellTemp" sheetId="3" r:id="rId3"/>
-    <sheet name="ActiveBpd" sheetId="4" r:id="rId4"/>
+    <sheet name="BpdAndRbc" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -17628,8 +17628,10 @@
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FFFFFFFF"/>
         <color rgb="FFFF6347"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF36C1FF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>